<commit_message>
added userstories & class diagram
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NanoNode-Nexus\NanoNode-Nexus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CC952D-3C68-466C-8E76-51D40D273E2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2C55E1-4CD1-411C-9ADB-444385F1F289}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="20715" windowHeight="13275" xr2:uid="{6E36DC40-5F18-4EBE-9BC3-7D855008A313}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Priority scale</t>
   </si>
@@ -93,6 +82,45 @@
   </si>
   <si>
     <t>Acceptance Criteria</t>
+  </si>
+  <si>
+    <t>Implementing classes for movable entities</t>
+  </si>
+  <si>
+    <t>Implementing classes for entities</t>
+  </si>
+  <si>
+    <t>Implementing classes for game-renderer</t>
+  </si>
+  <si>
+    <t>Implementing classes for stationary entities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementing classes for the rest of the derived entity classes </t>
+  </si>
+  <si>
+    <t>Implementing game class</t>
+  </si>
+  <si>
+    <t>Implementing database schema for save states</t>
+  </si>
+  <si>
+    <t>Implementing class for saving gamestate in DB</t>
+  </si>
+  <si>
+    <t>Implementing 1 aditional tower</t>
+  </si>
+  <si>
+    <t>Implementing class for Fog of War</t>
+  </si>
+  <si>
+    <t>Implementing one static game field</t>
+  </si>
+  <si>
+    <t>Implementing an algorithm for random game field generation</t>
+  </si>
+  <si>
+    <t>Implementing algorithm for pathfinding (A*)</t>
   </si>
 </sst>
 </file>
@@ -172,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -189,6 +217,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -244,8 +273,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{35383E86-7FBF-4BC5-A1FB-8B8878744FCB}" name="Tabelle1" displayName="Tabelle1" ref="C3:M36" totalsRowShown="0" dataDxfId="11">
-  <autoFilter ref="C3:M36" xr:uid="{35383E86-7FBF-4BC5-A1FB-8B8878744FCB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{35383E86-7FBF-4BC5-A1FB-8B8878744FCB}" name="Tabelle1" displayName="Tabelle1" ref="C3:M37" totalsRowShown="0" dataDxfId="11">
+  <autoFilter ref="C3:M37" xr:uid="{35383E86-7FBF-4BC5-A1FB-8B8878744FCB}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{25C8B47E-6BAC-4926-B248-911D3C771B26}" name="Priority" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{9CE9A60A-229A-4767-BF36-858767E4CC66}" name="BusinessValue" dataDxfId="9"/>
@@ -560,17 +589,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7C2921-B808-43C3-9286-7C3D73229528}">
-  <dimension ref="C1:M36"/>
+  <dimension ref="C1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C4:M19"/>
+      <selection activeCell="E16" sqref="E4:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="20.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" customWidth="1"/>
     <col min="7" max="7" width="29.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.28515625" customWidth="1"/>
@@ -657,8 +686,13 @@
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="D4" s="5"/>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -669,8 +703,13 @@
       <c r="M4" s="5"/>
     </row>
     <row r="5" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="D5" s="5"/>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -681,8 +720,13 @@
       <c r="M5" s="6"/>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="D6" s="5"/>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -693,8 +737,13 @@
       <c r="M6" s="6"/>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="D7" s="5"/>
+      <c r="E7" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -702,11 +751,16 @@
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
-      <c r="M7" s="7"/>
+      <c r="M7" s="6"/>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="5"/>
+      <c r="C8" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="D8" s="5"/>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -714,11 +768,16 @@
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="6"/>
+      <c r="M8" s="7"/>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="5"/>
+      <c r="C9" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="D9" s="5"/>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -729,8 +788,13 @@
       <c r="M9" s="6"/>
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="D10" s="5"/>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -741,8 +805,13 @@
       <c r="M10" s="6"/>
     </row>
     <row r="11" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="D11" s="5"/>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -753,8 +822,13 @@
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="D12" s="5"/>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
@@ -765,8 +839,13 @@
       <c r="M12" s="6"/>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="D13" s="5"/>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -777,8 +856,13 @@
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="D14" s="5"/>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -789,8 +873,13 @@
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="D15" s="5"/>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -801,8 +890,13 @@
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="D16" s="5"/>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -848,7 +942,7 @@
       <c r="L19" s="5"/>
       <c r="M19" s="6"/>
     </row>
-    <row r="20" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="F20" s="5"/>
@@ -858,7 +952,7 @@
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
+      <c r="M20" s="6"/>
     </row>
     <row r="21" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="5"/>
@@ -1052,12 +1146,24 @@
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
     </row>
+    <row r="37" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C36" xr:uid="{0C4E6ECF-68E6-4C69-84EC-B67BB79105BC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C37" xr:uid="{0C4E6ECF-68E6-4C69-84EC-B67BB79105BC}">
       <formula1>$D$1:$G$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D36" xr:uid="{CC98014D-015B-493D-AA10-1DCCCD92FE62}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D37" xr:uid="{CC98014D-015B-493D-AA10-1DCCCD92FE62}">
       <formula1>$D$2:$G$2</formula1>
     </dataValidation>
   </dataValidations>
@@ -1070,15 +1176,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0ba74dc7-3b53-4713-bb67-9e6187bc4572">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <a xmlns="0ba74dc7-3b53-4713-bb67-9e6187bc4572" xsi:nil="true"/>
-    <TaxCatchAll xmlns="b43d7674-e72d-422b-be95-e22e3af49d99" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1267,21 +1370,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0ba74dc7-3b53-4713-bb67-9e6187bc4572">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <a xmlns="0ba74dc7-3b53-4713-bb67-9e6187bc4572" xsi:nil="true"/>
+    <TaxCatchAll xmlns="b43d7674-e72d-422b-be95-e22e3af49d99" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE5B2139-0411-4F93-927B-CEF9303A0586}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3CD4954-40DF-4E1B-A417-8AC111E78ABB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0ba74dc7-3b53-4713-bb67-9e6187bc4572"/>
-    <ds:schemaRef ds:uri="b43d7674-e72d-422b-be95-e22e3af49d99"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1306,9 +1409,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3CD4954-40DF-4E1B-A417-8AC111E78ABB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE5B2139-0411-4F93-927B-CEF9303A0586}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0ba74dc7-3b53-4713-bb67-9e6187bc4572"/>
+    <ds:schemaRef ds:uri="b43d7674-e72d-422b-be95-e22e3af49d99"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>